<commit_message>
added patient match profile
</commit_message>
<xml_diff>
--- a/docs/0.1.0/StructureDefinition-alvearie-address.xlsx
+++ b/docs/0.1.0/StructureDefinition-alvearie-address.xlsx
@@ -231,7 +231,7 @@
     <t>countyCode</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://alvearie.github.io/alvearie-fhir-ig/StructureDefinition/county-code}
+    <t xml:space="preserve">Extension {http://alvearie.io/fhir/StructureDefinition/county-code}
 </t>
   </si>
   <si>
@@ -247,7 +247,7 @@
     <t>regionCode</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://alvearie.github.io/alvearie-fhir-ig/StructureDefinition/region-code}
+    <t xml:space="preserve">Extension {http://alvearie.io/fhir/StructureDefinition/region-code}
 </t>
   </si>
   <si>

</xml_diff>